<commit_message>
ajout de qql taches
</commit_message>
<xml_diff>
--- a/repartition des taches.xlsx
+++ b/repartition des taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EBA6FB4-9DD2-4205-9763-01D3FCED944B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE25706B-C4ED-4DF2-9069-7F01A949CF6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB517621-B655-4C83-B772-324F99E48A5A}"/>
   </bookViews>
@@ -29,6 +29,35 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Fonctionnalité</t>
+  </si>
+  <si>
+    <t>Utiliser les fonctionnalité du host en étant client</t>
+  </si>
+  <si>
+    <t>Pouvoir se connecter en tant que client/serveur</t>
+  </si>
+  <si>
+    <t>ne pas pouvoir utiliser les outils adverses</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>système client/socket</t>
+  </si>
+  <si>
+    <t>structure lancant une méthode</t>
+  </si>
+  <si>
+    <t>Système de propriétés</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,12 +407,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662EF6A4-89FA-462C-B31C-FFC213D9CC2E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>